<commit_message>
1. Upload bulk mappings 2. Improved caching with indexing
</commit_message>
<xml_diff>
--- a/incdocs-server/service/src/main/resources/bulk-upload-mapping.xlsx
+++ b/incdocs-server/service/src/main/resources/bulk-upload-mapping.xlsx
@@ -20,18 +20,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
   <si>
     <t xml:space="preserve">EmployeeID</t>
   </si>
   <si>
-    <t xml:space="preserve">CompanyID</t>
-  </si>
-  <si>
     <t xml:space="preserve">GroupHeadID</t>
   </si>
   <si>
     <t xml:space="preserve">Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pooja Sharma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poojash1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vishnubot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rahul Mane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rmane1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishnubotla Prasad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP_HEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sravya Prasad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sravya</t>
   </si>
 </sst>
 </file>
@@ -41,11 +74,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -67,6 +101,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF660E7A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,12 +155,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -129,6 +177,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660E7A"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -137,20 +245,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.03"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -162,6 +272,59 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>